<commit_message>
Notes update, generating slides
</commit_message>
<xml_diff>
--- a/docs/ServoCalibaration.xlsx
+++ b/docs/ServoCalibaration.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="570" windowWidth="24615" windowHeight="13680"/>
+    <workbookView xWindow="270" yWindow="570" windowWidth="24615" windowHeight="13680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="11" r:id="rId1"/>
-    <sheet name="Servo Data" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId3"/>
+    <sheet name="Curve" sheetId="12" r:id="rId2"/>
+    <sheet name="Servo Data" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -217,10 +218,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Servo Data'!$E$3:$E$65</c:f>
+              <c:f>'Servo Data'!$E$3:$E$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>-300</c:v>
                 </c:pt>
@@ -248,166 +249,166 @@
                 <c:pt idx="8">
                   <c:v>-220</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>-210</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>-200</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>-190</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>-180</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>-170</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>-160</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>-150</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>-140</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>-130</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>-120</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>-110</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>-100</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>-90</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>-80</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>-70</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>-60</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>-50</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>-40</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>-5</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="48">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="49">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="50">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="52">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>190</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="56">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="57">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="58">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="59">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="60">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="61">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="62">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="63">
                   <c:v>290</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="64">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -415,10 +416,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Servo Data'!$F$3:$F$65</c:f>
+              <c:f>'Servo Data'!$F$3:$F$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>1300</c:v>
                 </c:pt>
@@ -446,166 +447,166 @@
                 <c:pt idx="8">
                   <c:v>1427</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>1432</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>1437</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>1443</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>1448</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>1451</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>1453</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>1456</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>1458</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>1461</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>1463</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>1466</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>1468</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>1471</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>1474</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>1476</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>1479</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>1481</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>1484</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>1487</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>1489</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>1492</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>1498</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>1500</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>1502</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>1504</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>1506</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>1509</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>1512</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>1515</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>1518</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>1520</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>1523</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>1526</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>1529</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>1531</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>1534</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>1537</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="48">
                   <c:v>1539</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="49">
                   <c:v>1542</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="50">
                   <c:v>1545</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51">
                   <c:v>1547</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="52">
                   <c:v>1550</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>1556</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>1561</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>1567</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="56">
                   <c:v>1572</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="57">
                   <c:v>1578</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="58">
                   <c:v>1583</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="59">
                   <c:v>1589</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="60">
                   <c:v>1594</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="61">
                   <c:v>1600</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="62">
                   <c:v>1633</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="63">
                   <c:v>1667</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="64">
                   <c:v>1700</c:v>
                 </c:pt>
               </c:numCache>
@@ -632,10 +633,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Servo Data'!$E$3:$E$65</c:f>
+              <c:f>'Servo Data'!$E$3:$E$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>-300</c:v>
                 </c:pt>
@@ -663,166 +664,166 @@
                 <c:pt idx="8">
                   <c:v>-220</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>-210</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>-200</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>-190</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>-180</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>-170</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>-160</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>-150</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>-140</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>-130</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>-120</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>-110</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>-100</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>-90</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>-80</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>-70</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>-60</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>-50</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>-40</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>-5</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="48">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="49">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="50">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="52">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>190</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="56">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="57">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="58">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="59">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="60">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="61">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="62">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="63">
                   <c:v>290</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="64">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -830,10 +831,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Servo Data'!$G$3:$G$65</c:f>
+              <c:f>'Servo Data'!$G$3:$G$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>1300</c:v>
                 </c:pt>
@@ -861,17 +862,11 @@
                 <c:pt idx="8">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>1300</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1400</c:v>
@@ -898,10 +893,10 @@
                   <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1450</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1450</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>1450</c:v>
@@ -919,10 +914,10 @@
                   <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1475</c:v>
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1475</c:v>
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>1475</c:v>
@@ -931,19 +926,19 @@
                   <c:v>1475</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1525</c:v>
+                  <c:v>1475</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1525</c:v>
+                  <c:v>1475</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>1525</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1550</c:v>
+                  <c:v>1525</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1550</c:v>
+                  <c:v>1525</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>1550</c:v>
@@ -961,10 +956,10 @@
                   <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1600</c:v>
+                  <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1600</c:v>
+                  <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>1600</c:v>
@@ -991,10 +986,10 @@
                   <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1700</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1700</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>1700</c:v>
@@ -1021,6 +1016,12 @@
                   <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="62">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="64">
                   <c:v>1700</c:v>
                 </c:pt>
               </c:numCache>
@@ -1038,11 +1039,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42447872"/>
-        <c:axId val="47616512"/>
+        <c:axId val="43833344"/>
+        <c:axId val="68648256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42447872"/>
+        <c:axId val="43833344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1052,7 +1053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47616512"/>
+        <c:crossAx val="68648256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1060,7 +1061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47616512"/>
+        <c:axId val="68648256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1700"/>
@@ -1073,7 +1074,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42447872"/>
+        <c:crossAx val="43833344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1090,11 +1091,238 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.2764626570563723E-2"/>
+          <c:y val="8.4862308468857728E-2"/>
+          <c:w val="0.82945895254307478"/>
+          <c:h val="0.86461334557603897"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Servo Data'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pulse width (Micro seconds)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Servo Data'!$B$3:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-270</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-22.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-11.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Servo Data'!$A$3:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1474</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1483</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1489</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1491</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1492</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1508</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1509</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1511</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1517</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1526</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="51612672"/>
+        <c:axId val="47713664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="51612672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="47713664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="47713664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51612672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="174" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1102,6 +1330,33 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670774" cy="6297083"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -1415,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1453,14 +1708,15 @@
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>$A$10-(A17-$A$10)</f>
         <v>1400</v>
       </c>
       <c r="B3">
-        <f>-B9</f>
+        <f>-B17</f>
         <v>-270</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="0">B3/6</f>
+        <f t="shared" ref="C3:C5" si="0">B3/6</f>
         <v>-45</v>
       </c>
       <c r="E3" s="1">
@@ -1475,10 +1731,11 @@
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1448</v>
+        <f>$A$10-(A16-$A$10)</f>
+        <v>1450</v>
       </c>
       <c r="B4">
-        <f>-B8</f>
+        <f>-B16</f>
         <v>-180</v>
       </c>
       <c r="C4">
@@ -1497,10 +1754,11 @@
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1471</v>
+        <f>$A$10-(A15-$A$10)</f>
+        <v>1474</v>
       </c>
       <c r="B5">
-        <f>-B7</f>
+        <f>-B15</f>
         <v>-90</v>
       </c>
       <c r="C5">
@@ -1519,13 +1777,15 @@
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1500</v>
+        <f>$A$10-(A14-$A$10)</f>
+        <v>1483</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <f>-B14</f>
+        <v>-45</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>B10/6</f>
         <v>0</v>
       </c>
       <c r="E6" s="1">
@@ -1540,330 +1800,371 @@
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f>$A$10-(A13-$A$10)</f>
+        <v>1489</v>
+      </c>
+      <c r="B7">
+        <f>-B13</f>
+        <v>-22.5</v>
+      </c>
+      <c r="C7">
+        <f>B15/6</f>
+        <v>15</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-260</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1405</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>$A$10-(A12-$A$10)</f>
+        <v>1491</v>
+      </c>
+      <c r="B8">
+        <f>-B12</f>
+        <v>-15</v>
+      </c>
+      <c r="C8">
+        <f>B16/6</f>
+        <v>30</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-250</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1411</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>$A$10-(A11-$A$10)</f>
+        <v>1492</v>
+      </c>
+      <c r="B9">
+        <f>-B11</f>
+        <v>-11.25</v>
+      </c>
+      <c r="C9">
+        <f>B17/6</f>
+        <v>45</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-240</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1416</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1500</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-230</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1421</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1508</v>
+      </c>
+      <c r="B11">
+        <v>11.25</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-220</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1427</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1509</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1511</v>
+      </c>
+      <c r="B13">
+        <v>22.5</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1517</v>
+      </c>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-210</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1432</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>1526</v>
       </c>
-      <c r="B7">
+      <c r="B15">
         <f>(180/2)</f>
         <v>90</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-260</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1405</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="E15" s="1">
+        <v>-200</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1437</v>
+      </c>
+      <c r="G15" s="1">
         <v>1300</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>1550</v>
       </c>
-      <c r="B8">
+      <c r="B16">
         <f>360/2</f>
         <v>180</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-250</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1411</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="E16" s="2">
+        <v>-190</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1443</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>1600</v>
       </c>
-      <c r="B9">
+      <c r="B17">
         <f>(360 + 180) / 2</f>
         <v>270</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E9" s="1">
-        <v>-240</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1416</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="1">
-        <v>-230</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1421</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="1">
-        <v>-220</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1427</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="1">
-        <v>-210</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1432</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="1">
-        <v>-200</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1437</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="2">
-        <v>-190</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1443</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="2">
+      <c r="E17" s="2">
         <v>-180</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F17" s="2">
         <v>1448</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="2">
-        <v>-170</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1451</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="2">
-        <v>-160</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1453</v>
       </c>
       <c r="G17" s="2">
         <v>1400</v>
       </c>
     </row>
-    <row r="18" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18" s="2">
-        <v>-150</v>
+        <v>-170</v>
       </c>
       <c r="F18" s="2">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="G18" s="2">
         <v>1400</v>
       </c>
     </row>
-    <row r="19" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="2">
-        <v>-140</v>
+        <v>-160</v>
       </c>
       <c r="F19" s="2">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="G19" s="2">
         <v>1400</v>
       </c>
     </row>
-    <row r="20" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="2">
-        <v>-130</v>
+        <v>-150</v>
       </c>
       <c r="F20" s="2">
-        <v>1461</v>
+        <v>1456</v>
       </c>
       <c r="G20" s="2">
         <v>1400</v>
       </c>
     </row>
-    <row r="21" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="2">
-        <v>-120</v>
+        <v>-140</v>
       </c>
       <c r="F21" s="2">
-        <v>1463</v>
+        <v>1458</v>
       </c>
       <c r="G21" s="2">
         <v>1400</v>
       </c>
     </row>
-    <row r="22" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22" s="2">
-        <v>-110</v>
+        <v>-130</v>
       </c>
       <c r="F22" s="2">
-        <v>1466</v>
+        <v>1461</v>
       </c>
       <c r="G22" s="2">
         <v>1400</v>
       </c>
     </row>
-    <row r="23" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" s="2">
-        <v>-100</v>
+        <v>-120</v>
       </c>
       <c r="F23" s="2">
-        <v>1468</v>
+        <v>1463</v>
       </c>
       <c r="G23" s="2">
         <v>1400</v>
       </c>
     </row>
-    <row r="24" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="4">
+    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="2">
+        <v>-110</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1466</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="2">
+        <v>-100</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1468</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="4">
         <v>-90</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F26" s="4">
         <v>1471</v>
-      </c>
-      <c r="G24" s="4">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="25" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="4">
-        <v>-80</v>
-      </c>
-      <c r="F25" s="4">
-        <v>1474</v>
-      </c>
-      <c r="G25" s="4">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="26" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="4">
-        <v>-70</v>
-      </c>
-      <c r="F26" s="4">
-        <v>1476</v>
       </c>
       <c r="G26" s="4">
         <v>1450</v>
       </c>
     </row>
-    <row r="27" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="4">
-        <v>-60</v>
+        <v>-80</v>
       </c>
       <c r="F27" s="4">
-        <v>1479</v>
+        <v>1474</v>
       </c>
       <c r="G27" s="4">
         <v>1450</v>
       </c>
     </row>
-    <row r="28" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="4">
-        <v>-50</v>
+        <v>-70</v>
       </c>
       <c r="F28" s="4">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="G28" s="4">
         <v>1450</v>
       </c>
     </row>
-    <row r="29" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="4">
-        <v>-40</v>
+        <v>-60</v>
       </c>
       <c r="F29" s="4">
-        <v>1484</v>
+        <v>1479</v>
       </c>
       <c r="G29" s="4">
         <v>1450</v>
       </c>
     </row>
-    <row r="30" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="4">
-        <v>-30</v>
+        <v>-50</v>
       </c>
       <c r="F30" s="4">
-        <v>1487</v>
+        <v>1481</v>
       </c>
       <c r="G30" s="4">
         <v>1450</v>
       </c>
     </row>
-    <row r="31" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="5">
+    <row r="31" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="4">
+        <v>-40</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1484</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="4">
+        <v>-30</v>
+      </c>
+      <c r="F32" s="4">
+        <v>1487</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="5">
         <v>-20</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F33" s="5">
         <v>1489</v>
-      </c>
-      <c r="G31" s="3">
-        <v>1475</v>
-      </c>
-    </row>
-    <row r="32" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E32" s="3">
-        <v>-10</v>
-      </c>
-      <c r="F32" s="3">
-        <v>1492</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1475</v>
-      </c>
-    </row>
-    <row r="33" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="3">
-        <v>5</v>
-      </c>
-      <c r="F33" s="3">
-        <f>F32 +(F36-F32)/2</f>
-        <v>1498</v>
       </c>
       <c r="G33" s="3">
         <v>1475</v>
@@ -1871,10 +2172,10 @@
     </row>
     <row r="34" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="3">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="F34" s="3">
-        <v>1500</v>
+        <v>1492</v>
       </c>
       <c r="G34" s="3">
         <v>1475</v>
@@ -1882,66 +2183,67 @@
     </row>
     <row r="35" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="3">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="F35" s="3">
-        <f>F34 +(F36-F34)/2</f>
-        <v>1502</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1525</v>
+        <f>F34 +(F38-F34)/2</f>
+        <v>1498</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1475</v>
       </c>
     </row>
     <row r="36" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F36" s="3">
-        <v>1504</v>
-      </c>
-      <c r="G36" s="5">
-        <v>1525</v>
+        <v>1500</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1475</v>
       </c>
     </row>
     <row r="37" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E37" s="5">
-        <v>20</v>
-      </c>
-      <c r="F37" s="5">
-        <v>1506</v>
+      <c r="E37" s="3">
+        <v>-5</v>
+      </c>
+      <c r="F37" s="3">
+        <f>F36 +(F38-F36)/2</f>
+        <v>1502</v>
       </c>
       <c r="G37" s="5">
         <v>1525</v>
       </c>
     </row>
     <row r="38" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E38" s="4">
-        <v>30</v>
-      </c>
-      <c r="F38" s="4">
-        <v>1509</v>
-      </c>
-      <c r="G38" s="4">
-        <v>1550</v>
+      <c r="E38" s="3">
+        <v>10</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1504</v>
+      </c>
+      <c r="G38" s="5">
+        <v>1525</v>
       </c>
     </row>
     <row r="39" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E39" s="4">
-        <v>40</v>
-      </c>
-      <c r="F39" s="4">
-        <v>1512</v>
-      </c>
-      <c r="G39" s="4">
-        <v>1550</v>
+      <c r="E39" s="5">
+        <v>20</v>
+      </c>
+      <c r="F39" s="5">
+        <v>1506</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1525</v>
       </c>
     </row>
     <row r="40" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40" s="4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F40" s="4">
-        <v>1515</v>
+        <v>1509</v>
       </c>
       <c r="G40" s="4">
         <v>1550</v>
@@ -1949,10 +2251,10 @@
     </row>
     <row r="41" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="4">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F41" s="4">
-        <v>1518</v>
+        <v>1512</v>
       </c>
       <c r="G41" s="4">
         <v>1550</v>
@@ -1960,10 +2262,10 @@
     </row>
     <row r="42" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" s="4">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F42" s="4">
-        <v>1520</v>
+        <v>1515</v>
       </c>
       <c r="G42" s="4">
         <v>1550</v>
@@ -1971,10 +2273,10 @@
     </row>
     <row r="43" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E43" s="4">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F43" s="4">
-        <v>1523</v>
+        <v>1518</v>
       </c>
       <c r="G43" s="4">
         <v>1550</v>
@@ -1982,43 +2284,43 @@
     </row>
     <row r="44" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E44" s="4">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F44" s="4">
-        <v>1526</v>
+        <v>1520</v>
       </c>
       <c r="G44" s="4">
         <v>1550</v>
       </c>
     </row>
     <row r="45" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="2">
+      <c r="E45" s="4">
+        <v>80</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1523</v>
+      </c>
+      <c r="G45" s="4">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="4">
+        <v>90</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1526</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="2">
         <v>100</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F47" s="2">
         <v>1529</v>
-      </c>
-      <c r="G45" s="2">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="46" spans="5:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="E46" s="2">
-        <v>110</v>
-      </c>
-      <c r="F46" s="2">
-        <v>1531</v>
-      </c>
-      <c r="G46" s="2">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="47" spans="5:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="E47" s="2">
-        <v>120</v>
-      </c>
-      <c r="F47" s="2">
-        <v>1534</v>
       </c>
       <c r="G47" s="2">
         <v>1600</v>
@@ -2026,10 +2328,10 @@
     </row>
     <row r="48" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E48" s="2">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="F48" s="2">
-        <v>1537</v>
+        <v>1531</v>
       </c>
       <c r="G48" s="2">
         <v>1600</v>
@@ -2037,10 +2339,10 @@
     </row>
     <row r="49" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E49" s="2">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F49" s="2">
-        <v>1539</v>
+        <v>1534</v>
       </c>
       <c r="G49" s="2">
         <v>1600</v>
@@ -2048,10 +2350,10 @@
     </row>
     <row r="50" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E50" s="2">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="F50" s="2">
-        <v>1542</v>
+        <v>1537</v>
       </c>
       <c r="G50" s="2">
         <v>1600</v>
@@ -2059,10 +2361,10 @@
     </row>
     <row r="51" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E51" s="2">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="F51" s="2">
-        <v>1545</v>
+        <v>1539</v>
       </c>
       <c r="G51" s="2">
         <v>1600</v>
@@ -2070,10 +2372,10 @@
     </row>
     <row r="52" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E52" s="2">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="F52" s="2">
-        <v>1547</v>
+        <v>1542</v>
       </c>
       <c r="G52" s="2">
         <v>1600</v>
@@ -2081,10 +2383,10 @@
     </row>
     <row r="53" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E53" s="2">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="F53" s="2">
-        <v>1550</v>
+        <v>1545</v>
       </c>
       <c r="G53" s="2">
         <v>1600</v>
@@ -2092,43 +2394,43 @@
     </row>
     <row r="54" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E54" s="2">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="F54" s="2">
-        <v>1556</v>
+        <v>1547</v>
       </c>
       <c r="G54" s="2">
         <v>1600</v>
       </c>
     </row>
     <row r="55" spans="5:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="E55" s="1">
-        <v>200</v>
-      </c>
-      <c r="F55" s="1">
-        <v>1561</v>
-      </c>
-      <c r="G55" s="1">
-        <v>1700</v>
+      <c r="E55" s="2">
+        <v>180</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1550</v>
+      </c>
+      <c r="G55" s="2">
+        <v>1600</v>
       </c>
     </row>
     <row r="56" spans="5:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="E56" s="1">
-        <v>210</v>
-      </c>
-      <c r="F56" s="1">
-        <v>1567</v>
-      </c>
-      <c r="G56" s="1">
-        <v>1700</v>
+      <c r="E56" s="2">
+        <v>190</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1556</v>
+      </c>
+      <c r="G56" s="2">
+        <v>1600</v>
       </c>
     </row>
     <row r="57" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E57" s="1">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="F57" s="1">
-        <v>1572</v>
+        <v>1561</v>
       </c>
       <c r="G57" s="1">
         <v>1700</v>
@@ -2136,10 +2438,10 @@
     </row>
     <row r="58" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E58" s="1">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="F58" s="1">
-        <v>1578</v>
+        <v>1567</v>
       </c>
       <c r="G58" s="1">
         <v>1700</v>
@@ -2147,10 +2449,10 @@
     </row>
     <row r="59" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E59" s="1">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="F59" s="1">
-        <v>1583</v>
+        <v>1572</v>
       </c>
       <c r="G59" s="1">
         <v>1700</v>
@@ -2158,10 +2460,10 @@
     </row>
     <row r="60" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E60" s="1">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="F60" s="1">
-        <v>1589</v>
+        <v>1578</v>
       </c>
       <c r="G60" s="1">
         <v>1700</v>
@@ -2169,10 +2471,10 @@
     </row>
     <row r="61" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E61" s="1">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="F61" s="1">
-        <v>1594</v>
+        <v>1583</v>
       </c>
       <c r="G61" s="1">
         <v>1700</v>
@@ -2180,10 +2482,10 @@
     </row>
     <row r="62" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E62" s="1">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="F62" s="1">
-        <v>1600</v>
+        <v>1589</v>
       </c>
       <c r="G62" s="1">
         <v>1700</v>
@@ -2191,34 +2493,56 @@
     </row>
     <row r="63" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E63" s="1">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="F63" s="1">
-        <v>1633</v>
+        <v>1594</v>
       </c>
       <c r="G63" s="1">
         <v>1700</v>
       </c>
     </row>
-    <row r="64" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E64" s="1">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="F64" s="1">
-        <v>1667</v>
+        <v>1600</v>
       </c>
       <c r="G64" s="1">
         <v>1700</v>
       </c>
     </row>
-    <row r="65" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E65" s="1">
+        <v>280</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1633</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E66" s="1">
+        <v>290</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1667</v>
+      </c>
+      <c r="G66" s="1">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="1">
         <v>300</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F67" s="1">
         <v>1700</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G67" s="1">
         <v>1700</v>
       </c>
     </row>

</xml_diff>